<commit_message>
Revert "Merge remote-tracking branch 'origin/Dev_0.0.1' into ArtWork"
This reverts commit a6bbc100c5552763757e2907bba0d80535ac7db3, reversing
changes made to 096ddf5aaef57efee3a6175dc5f7e4e7dd6a089e.
</commit_message>
<xml_diff>
--- a/truck/Table/Character.xlsx
+++ b/truck/Table/Character.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\truckproject\kci\truck\Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kci\kci\truck\Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0CA52-0459-4429-9DD2-460C4AD55F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CA724A-EB21-4578-A7C0-8AB33B24A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="390" windowWidth="25560" windowHeight="14685" xr2:uid="{E13B9AA5-2A18-43E8-8D01-C8614F668F08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E13B9AA5-2A18-43E8-8D01-C8614F668F08}"/>
   </bookViews>
   <sheets>
     <sheet name="#Character" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>long</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,7 +98,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>할아버지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>스페셜몬스터 태그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잼민이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -108,40 +116,6 @@
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mon1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mon2</t>
-  </si>
-  <si>
-    <t>Mob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mon1_desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mon2_desc</t>
-  </si>
-  <si>
-    <t>mon3</t>
-  </si>
-  <si>
-    <t>mon4</t>
-  </si>
-  <si>
-    <t>mon3_desc</t>
-  </si>
-  <si>
-    <t>mon4_desc</t>
-  </si>
-  <si>
-    <t>mon1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -568,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C17399B-D4C3-4AB1-B3D3-2D958F901435}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -636,24 +610,24 @@
         <v>10</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -668,83 +642,46 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reapply "Merge remote-tracking branch 'origin/Dev_0.0.1' into ArtWork"
This reverts commit a18852a047a3dcc8b11d28369ec13e37f723f58c.
</commit_message>
<xml_diff>
--- a/truck/Table/Character.xlsx
+++ b/truck/Table/Character.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kci\kci\truck\Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\truckproject\kci\truck\Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CA724A-EB21-4578-A7C0-8AB33B24A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0CA52-0459-4429-9DD2-460C4AD55F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E13B9AA5-2A18-43E8-8D01-C8614F668F08}"/>
+    <workbookView xWindow="975" yWindow="390" windowWidth="25560" windowHeight="14685" xr2:uid="{E13B9AA5-2A18-43E8-8D01-C8614F668F08}"/>
   </bookViews>
   <sheets>
     <sheet name="#Character" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>long</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,15 +98,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>할아버지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스페셜몬스터 태그</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잼민이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -116,6 +108,40 @@
   </si>
   <si>
     <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mon1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mon2</t>
+  </si>
+  <si>
+    <t>Mob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mon1_desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mon2_desc</t>
+  </si>
+  <si>
+    <t>mon3</t>
+  </si>
+  <si>
+    <t>mon4</t>
+  </si>
+  <si>
+    <t>mon3_desc</t>
+  </si>
+  <si>
+    <t>mon4_desc</t>
+  </si>
+  <si>
+    <t>mon1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -542,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C17399B-D4C3-4AB1-B3D3-2D958F901435}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -610,24 +636,24 @@
         <v>10</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -642,46 +668,83 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="b">
         <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="b">
         <v>0</v>
       </c>
-      <c r="I5">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="b">
         <v>0</v>
       </c>
-      <c r="J5" t="b">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>